<commit_message>
fixed invalid react hooks
</commit_message>
<xml_diff>
--- a/public/data/leaderboard.xlsx
+++ b/public/data/leaderboard.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -28,6 +28,12 @@
     <t>Date</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t>20/05/2025</t>
+  </si>
+  <si>
     <t>S</t>
   </si>
   <si>
@@ -35,6 +41,12 @@
   </si>
   <si>
     <t>19/05/2025</t>
+  </si>
+  <si>
+    <t>ssssssss</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -1186,7 +1198,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -1215,15 +1227,90 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>257</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>227</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>115</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>102</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1">
         <v>96</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1">
+        <v>49</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>

<commit_message>
fixed bugs with saving files
</commit_message>
<xml_diff>
--- a/public/data/leaderboard.xlsx
+++ b/public/data/leaderboard.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -28,25 +28,60 @@
     <t>Date</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>20/05/2025</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>s@d.com</t>
-  </si>
-  <si>
-    <t>19/05/2025</t>
-  </si>
-  <si>
-    <t>ssssssss</t>
-  </si>
-  <si>
-    <t>s</t>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>b@bbbbbb.com</t>
+  </si>
+  <si>
+    <t>SSSSSSS</t>
+  </si>
+  <si>
+    <t>s@s.com</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>ADSGADFASDFASDFSA</t>
+  </si>
+  <si>
+    <t>a@d.com</t>
+  </si>
+  <si>
+    <t>Winner</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <color indexed="12"/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>aga@aga.com</t>
+    </r>
+  </si>
+  <si>
+    <t>sK</t>
+  </si>
+  <si>
+    <t>aaaa@a.xom</t>
+  </si>
+  <si>
+    <t>ghjgfjhfgjh</t>
+  </si>
+  <si>
+    <t>vvfhgfh@h.com</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>d@d.com</t>
   </si>
 </sst>
 </file>
@@ -141,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="bottom"/>
@@ -154,6 +189,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1198,7 +1236,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -1222,97 +1260,205 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" ht="14.7" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1">
-        <v>257</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>300</v>
+      </c>
+      <c r="D2" s="5">
+        <v>45796.38566594907</v>
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" ht="13.55" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1">
-        <v>227</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>280</v>
+      </c>
+      <c r="D3" s="5">
+        <v>45796.38566594907</v>
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" ht="13.55" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1">
-        <v>115</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="D4" s="5">
+        <v>45796.38566594907</v>
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" ht="13.55" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1">
-        <v>102</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="D5" s="5">
+        <v>45796.38566594907</v>
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" ht="13.55" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1">
-        <v>96</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
+      </c>
+      <c r="D6" s="5">
+        <v>45796.38566594907</v>
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" ht="13.55" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1">
-        <v>49</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="D7" s="5">
+        <v>45796.38566594907</v>
       </c>
       <c r="E7" s="1"/>
     </row>
+    <row r="8" ht="13.55" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1">
+        <v>10</v>
+      </c>
+      <c r="D8" s="5">
+        <v>45796.38566594907</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5">
+        <v>45796.38566594907</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5">
+        <v>45796.38566594907</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" ht="13.55" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1">
+        <v>9</v>
+      </c>
+      <c r="D11" s="5">
+        <v>45796.38566594907</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" ht="13.55" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>45796.38566594907</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" ht="13.55" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>45796.38566594907</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" ht="13.55" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>45796.38566594907</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B11" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="72" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
   <headerFooter>

</xml_diff>